<commit_message>
Cập nhật bài tập về Newton, thêm file dữ liệu và ảnh\
</commit_message>
<xml_diff>
--- a/TH Excel/3. Nội suy Newton/Nội suy Newton.xlsx
+++ b/TH Excel/3. Nội suy Newton/Nội suy Newton.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtien\Desktop\PPS\Tien\3. Nội suy Newton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Hust\Numerical Analysis\TH Excel\3. Nội suy Newton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4436B8F0-7804-46A5-A71C-7D80936D8763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FA797B-7D88-4B2C-B003-0A0435914912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{33690276-A90C-4337-B0B3-5AE93AEA16A0}"/>
+    <workbookView xWindow="15075" yWindow="3765" windowWidth="13830" windowHeight="10995" activeTab="3" xr2:uid="{33690276-A90C-4337-B0B3-5AE93AEA16A0}"/>
   </bookViews>
   <sheets>
     <sheet name="6 mốc" sheetId="4" r:id="rId1"/>
@@ -143,7 +143,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -151,20 +151,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -172,7 +172,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -691,17 +691,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA025622-8076-4324-822B-6213A7A9FF90}">
   <dimension ref="B2:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.25" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>22</v>
       </c>
@@ -724,7 +724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C3" s="2">
         <v>1.57</v>
       </c>
@@ -733,7 +733,7 @@
         <v>2.4624999999999999</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C4" s="5">
         <v>1.59</v>
       </c>
@@ -746,7 +746,7 @@
         <v>6.1600000000000046</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C5" s="5">
         <v>1.62</v>
       </c>
@@ -763,7 +763,7 @@
         <v>0.999999999999587</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C6" s="5">
         <v>1.64</v>
       </c>
@@ -784,7 +784,7 @@
         <v>-2.8571428571140736</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C7" s="5">
         <v>1.67</v>
       </c>
@@ -809,7 +809,7 @@
         <v>53.571428570771808</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="7">
         <v>1.71</v>
       </c>
@@ -841,7 +841,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -850,7 +850,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>6</v>
       </c>
@@ -880,8 +880,8 @@
       </c>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -904,7 +904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D14" cm="1">
         <f t="array" ref="D14:D18">C3:C7</f>
         <v>1.57</v>
@@ -929,7 +929,7 @@
         <v>-1.57</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D15">
         <v>1.59</v>
       </c>
@@ -953,7 +953,7 @@
         <v>2.4963000000000002</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D16">
         <v>1.62</v>
       </c>
@@ -977,7 +977,7 @@
         <v>-4.0440060000000004</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D17">
         <v>1.64</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>6.6321698400000004</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D18">
         <v>1.67</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>-11.075723632800001</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>7</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>7294.9285776137694</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>19</v>
       </c>
@@ -1082,8 +1082,8 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="24" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>9</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D26">
         <f>C8</f>
         <v>1.71</v>
@@ -1131,7 +1131,7 @@
         <v>-1.71</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D27">
         <f>C7</f>
         <v>1.67</v>
@@ -1156,7 +1156,7 @@
         <v>2.8556999999999997</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D28">
         <f>C6</f>
         <v>1.64</v>
@@ -1181,7 +1181,7 @@
         <v>-4.6833479999999996</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D29">
         <f>C5</f>
         <v>1.62</v>
@@ -1206,7 +1206,7 @@
         <v>7.5870237600000001</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D30">
         <f>C4</f>
         <v>1.59</v>
@@ -1231,12 +1231,12 @@
         <v>-12.0633677784</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="E33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>11</v>
       </c>
@@ -1274,13 +1274,13 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.25" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>22</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C3" s="2">
         <v>1.57</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>2.4624999999999999</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C4" s="5">
         <v>1.59</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>6.1600000000000046</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C5" s="5">
         <v>1.62</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>0.999999999999587</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C6" s="5">
         <v>1.64</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>-2.8571428571140736</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C7" s="5">
         <v>1.67</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>53.571428570771808</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="5">
         <v>1.71</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>-625.94482236564352</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="7">
         <v>1.74</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>6</v>
       </c>
@@ -1489,8 +1489,8 @@
         <v>5225.2382433788107</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D14" cm="1">
         <f t="array" ref="D14:D19">C3:C8</f>
         <v>1.57</v>
@@ -1544,7 +1544,7 @@
         <v>-1.57</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D15">
         <v>1.59</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>2.4963000000000002</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D16">
         <v>1.62</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>-4.0440060000000004</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D17">
         <v>1.64</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>6.6321698400000004</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D18">
         <v>1.67</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>-11.075723632800001</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>1.71</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>18.939487412088003</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>7</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>106258.26251324758</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>19</v>
       </c>
@@ -1742,8 +1742,8 @@
         <v>2.8970000002591405</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="E24" s="2">
         <v>0</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>9</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>-1.74</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D26">
         <f>C8</f>
         <v>1.71</v>
@@ -1825,7 +1825,7 @@
         <v>2.9754</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D27">
         <f>C7</f>
         <v>1.67</v>
@@ -1853,7 +1853,7 @@
         <v>-4.9689179999999995</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D28">
         <f>C6</f>
         <v>1.64</v>
@@ -1881,7 +1881,7 @@
         <v>8.1490255199999986</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D29">
         <f>C5</f>
         <v>1.62</v>
@@ -1909,7 +1909,7 @@
         <v>-13.201421342399998</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D30">
         <f>C4</f>
         <v>1.59</v>
@@ -1937,12 +1937,12 @@
         <v>20.990259934415999</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="E33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>11</v>
       </c>
@@ -1984,12 +1984,12 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="21.7265625" customWidth="1"/>
+    <col min="3" max="3" width="21.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>22</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="2">
         <v>0.3</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>-0.73899999999999999</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="5">
         <v>0.6</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>1.7500000000000002</v>
       </c>
     </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="5">
         <v>0.8</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>16.839999999999996</v>
       </c>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="5">
         <v>0.9</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>16.377777777777812</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="5">
         <v>1.2</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>4.3333333333332806</v>
       </c>
     </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="5">
         <v>1.4</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>8.207070707078612E-2</v>
       </c>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="5">
         <v>1.7</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>-7.5156325156438039E-2</v>
       </c>
     </row>
-    <row r="10" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="7">
         <v>1.9</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:13" ht="15" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>13</v>
       </c>
@@ -2239,8 +2239,8 @@
         <v>3.4456284456502985E-2</v>
       </c>
     </row>
-    <row r="13" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>14</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="D15" cm="1">
         <f t="array" ref="D15:D21">C3:C9</f>
         <v>0.3</v>
@@ -2300,7 +2300,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="D16">
         <v>0.6</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D17">
         <v>0.8</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>-0.14399999999999999</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D18">
         <v>0.9</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>0.12959999999999999</v>
       </c>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D19">
         <v>1.2</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>-0.15551999999999999</v>
       </c>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D20">
         <v>1.4</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>0.21772799999999998</v>
       </c>
     </row>
-    <row r="21" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D21">
         <v>1.7</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>-0.37013759999999996</v>
       </c>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>15</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>-7.1480839160969534E-2</v>
       </c>
     </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>16</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>6.1424858275058254</v>
       </c>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>17</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>28.920449063899063</v>
       </c>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>18</v>
       </c>
@@ -2622,8 +2622,8 @@
         <v>81.720801217301215</v>
       </c>
     </row>
-    <row r="30" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>21</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D32">
         <f>C10</f>
         <v>1.9</v>
@@ -2683,7 +2683,7 @@
         <v>-1.9</v>
       </c>
     </row>
-    <row r="33" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:13" x14ac:dyDescent="0.2">
       <c r="D33">
         <f>C9</f>
         <v>1.7</v>
@@ -2714,7 +2714,7 @@
         <v>3.23</v>
       </c>
     </row>
-    <row r="34" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:13" x14ac:dyDescent="0.2">
       <c r="D34">
         <f>C8</f>
         <v>1.4</v>
@@ -2745,7 +2745,7 @@
         <v>-4.5219999999999994</v>
       </c>
     </row>
-    <row r="35" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:13" x14ac:dyDescent="0.2">
       <c r="D35">
         <f>C7</f>
         <v>1.2</v>
@@ -2776,7 +2776,7 @@
         <v>5.4263999999999992</v>
       </c>
     </row>
-    <row r="36" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:13" x14ac:dyDescent="0.2">
       <c r="D36">
         <f>C6</f>
         <v>0.9</v>
@@ -2807,7 +2807,7 @@
         <v>-4.8837599999999997</v>
       </c>
     </row>
-    <row r="37" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:13" x14ac:dyDescent="0.2">
       <c r="D37">
         <f>C5</f>
         <v>0.8</v>
@@ -2838,7 +2838,7 @@
         <v>3.9070079999999998</v>
       </c>
     </row>
-    <row r="38" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D38">
         <f>C4</f>
         <v>0.6</v>
@@ -2869,7 +2869,7 @@
         <v>-2.3442048</v>
       </c>
     </row>
-    <row r="41" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
         <v>11</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>-7.1480839160951506E-2</v>
       </c>
     </row>
-    <row r="42" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:13" ht="15" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>16</v>
       </c>
@@ -2940,7 +2940,7 @@
       </c>
       <c r="M42" s="15"/>
     </row>
-    <row r="43" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:13" ht="15" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>17</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>28.920449063899071</v>
       </c>
     </row>
-    <row r="44" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:13" ht="15" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>18</v>
       </c>
@@ -3028,16 +3028,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47A58F4-2CCE-4BFA-B765-5BE166C0E80B}">
   <dimension ref="C2:N44"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="C24" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="19.453125" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>22</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C3" s="2">
         <v>0.3</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>-0.73899999999999999</v>
       </c>
     </row>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C4" s="5">
         <v>0.6</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>1.7500000000000002</v>
       </c>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C5" s="5">
         <v>0.8</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>16.839999999999996</v>
       </c>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C6" s="5">
         <v>0.9</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>16.377777777777812</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C7" s="5">
         <v>1.2</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>4.3333333333332806</v>
       </c>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C8" s="5">
         <v>1.4</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>8.207070707078612E-2</v>
       </c>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C9" s="5">
         <v>1.7</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>-7.5156325156438039E-2</v>
       </c>
     </row>
-    <row r="10" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C10" s="5">
         <v>1.9</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>3.4456284456502985E-2</v>
       </c>
     </row>
-    <row r="11" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="7">
         <v>2.2000000000000002</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
@@ -3332,8 +3332,8 @@
         <v>8.1850410793175652E-3</v>
       </c>
     </row>
-    <row r="13" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>14</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D15" cm="1">
         <f t="array" ref="D15:D22">C3:C10</f>
         <v>0.3</v>
@@ -3399,7 +3399,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D16">
         <v>0.6</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D17">
         <v>0.8</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>-0.14399999999999999</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D18">
         <v>0.9</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>0.12959999999999999</v>
       </c>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D19">
         <v>1.2</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>-0.15551999999999999</v>
       </c>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D20">
         <v>1.4</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>0.21772799999999998</v>
       </c>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D21">
         <v>1.7</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>-0.37013759999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D22">
         <v>1.9</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>0.7032614399999999</v>
       </c>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>15</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>-6.5724615385069504E-2</v>
       </c>
     </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>16</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>6.1424881376518208</v>
       </c>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>17</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>28.920469598530126</v>
       </c>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>18</v>
       </c>
@@ -3791,8 +3791,8 @@
         <v>81.720596067431615</v>
       </c>
     </row>
-    <row r="30" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>21</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D32">
         <f>C11</f>
         <v>2.2000000000000002</v>
@@ -3858,7 +3858,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="33" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:13" x14ac:dyDescent="0.2">
       <c r="D33">
         <f>C10</f>
         <v>1.9</v>
@@ -3892,7 +3892,7 @@
         <v>4.18</v>
       </c>
     </row>
-    <row r="34" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:13" x14ac:dyDescent="0.2">
       <c r="D34">
         <f>C9</f>
         <v>1.7</v>
@@ -3926,7 +3926,7 @@
         <v>-7.105999999999999</v>
       </c>
     </row>
-    <row r="35" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:13" x14ac:dyDescent="0.2">
       <c r="D35">
         <f>C8</f>
         <v>1.4</v>
@@ -3960,7 +3960,7 @@
         <v>9.9483999999999977</v>
       </c>
     </row>
-    <row r="36" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:13" x14ac:dyDescent="0.2">
       <c r="D36">
         <f>C7</f>
         <v>1.2</v>
@@ -3994,7 +3994,7 @@
         <v>-11.938079999999998</v>
       </c>
     </row>
-    <row r="37" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:13" x14ac:dyDescent="0.2">
       <c r="D37">
         <f>C6</f>
         <v>0.9</v>
@@ -4028,7 +4028,7 @@
         <v>10.744271999999999</v>
       </c>
     </row>
-    <row r="38" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:13" x14ac:dyDescent="0.2">
       <c r="D38">
         <f>C5</f>
         <v>0.8</v>
@@ -4062,7 +4062,7 @@
         <v>-8.5954175999999993</v>
       </c>
     </row>
-    <row r="39" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D39">
         <f>C4</f>
         <v>0.6</v>
@@ -4096,7 +4096,7 @@
         <v>5.1572505599999996</v>
       </c>
     </row>
-    <row r="41" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
         <v>11</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>-6.5724615385051186E-2</v>
       </c>
     </row>
-    <row r="42" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:13" ht="15" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>16</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>6.1424881376517622</v>
       </c>
     </row>
-    <row r="43" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:13" ht="15" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>17</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>28.920469598530055</v>
       </c>
     </row>
-    <row r="44" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:13" ht="15" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>18</v>
       </c>

</xml_diff>